<commit_message>
Additional Changes for repo
</commit_message>
<xml_diff>
--- a/UpdateCourseOfferingCourseOfferingTemplate.xlsx
+++ b/UpdateCourseOfferingCourseOfferingTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Venkat\Source\ExcelUpload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4738218D-4923-4AB9-A266-C9AA2E6F8874}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C18B32-B905-447A-BDCD-272AB0001259}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="7590" activeTab="1" xr2:uid="{DC0DE665-DC5B-4E82-A28B-EA52864D6C96}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="7590" firstSheet="2" activeTab="1" xr2:uid="{DC0DE665-DC5B-4E82-A28B-EA52864D6C96}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>All the Date format must be in DD/MM/YYYY Format</t>
   </si>
@@ -58,108 +58,111 @@
     <t>CourseTitle</t>
   </si>
   <si>
+    <t>MinEnrolled</t>
+  </si>
+  <si>
+    <t>MaxEnrolled</t>
+  </si>
+  <si>
+    <t>PriceGroupId</t>
+  </si>
+  <si>
+    <t>CourseLevelId</t>
+  </si>
+  <si>
+    <t>EnrollmentModeId</t>
+  </si>
+  <si>
+    <t>CR6G6Z1015A</t>
+  </si>
+  <si>
+    <t>Computing Placement</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>PriceGroup.PriceGroup78</t>
+  </si>
+  <si>
+    <t>CourseLevel.Placement</t>
+  </si>
+  <si>
+    <t>CourseEnrolMode.UGPlaceholder</t>
+  </si>
+  <si>
+    <t>CR6G6Z1101A</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>PriceGroup.PriceGroup48</t>
+  </si>
+  <si>
+    <t>CourseLevel.FHEQLevel6</t>
+  </si>
+  <si>
+    <t>CR6G6Z1103A</t>
+  </si>
+  <si>
+    <t>Enterprise Programming</t>
+  </si>
+  <si>
+    <t>PriceGroup.PriceGroup52</t>
+  </si>
+  <si>
+    <t>CR6G6Z1104A</t>
+  </si>
+  <si>
+    <t>Mobile Applications Development</t>
+  </si>
+  <si>
+    <t>CR6G6Z1105A</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>API Reference</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Reason for failure</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>AcademicPeriod</t>
+  </si>
+  <si>
     <t>StartDate</t>
   </si>
   <si>
     <t>EndDate</t>
   </si>
   <si>
-    <t>MinEnrolled</t>
-  </si>
-  <si>
-    <t>MaxEnrolled</t>
-  </si>
-  <si>
-    <t>PriceGroupId</t>
-  </si>
-  <si>
-    <t>CourseLevelId</t>
-  </si>
-  <si>
-    <t>EnrollmentModeId</t>
-  </si>
-  <si>
-    <t>CR6G6Z1015A</t>
-  </si>
-  <si>
-    <t>Computing Placement</t>
+    <t>CourselevelId</t>
+  </si>
+  <si>
+    <t>CR6G6Z1113A</t>
+  </si>
+  <si>
+    <t>AcademicPeriod.2018September</t>
+  </si>
+  <si>
+    <t>Network and Internet Forensics</t>
   </si>
   <si>
     <t>NULL</t>
   </si>
   <si>
-    <t>PriceGroup.PriceGroup78</t>
-  </si>
-  <si>
-    <t>CourseLevel.Placement</t>
-  </si>
-  <si>
-    <t>CourseEnrolMode.UGPlaceholder</t>
-  </si>
-  <si>
-    <t>CR6G6Z1101A</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>PriceGroup.PriceGroup48</t>
-  </si>
-  <si>
-    <t>CourseLevel.FHEQLevel6</t>
-  </si>
-  <si>
-    <t>CR6G6Z1103A</t>
-  </si>
-  <si>
-    <t>Enterprise Programming</t>
-  </si>
-  <si>
-    <t>PriceGroup.PriceGroup52</t>
-  </si>
-  <si>
-    <t>CR6G6Z1104A</t>
-  </si>
-  <si>
-    <t>Mobile Applications Development</t>
-  </si>
-  <si>
-    <t>CR6G6Z1105A</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>API Reference</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>Reason for failure</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>AcademicPeriod</t>
-  </si>
-  <si>
-    <t>CourselevelId</t>
-  </si>
-  <si>
-    <t>CR6G6Z1113A</t>
-  </si>
-  <si>
-    <t>AcademicPeriod.2018September</t>
-  </si>
-  <si>
-    <t>Network and Internet Forensics</t>
-  </si>
-  <si>
     <t>AcademicPeriod.2019September</t>
   </si>
   <si>
@@ -187,10 +190,7 @@
     <t>Result</t>
   </si>
   <si>
-    <t>Reason</t>
-  </si>
-  <si>
-    <t>"01/08/2020"</t>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -340,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -363,9 +363,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -375,7 +372,118 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -542,9 +650,7 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -579,9 +685,7 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -653,7 +757,9 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -688,191 +794,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -900,21 +821,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD3A9504-19FF-431D-AD02-E3A18E1E6005}" name="Table4" displayName="Table4" ref="B2:M7" totalsRowShown="0">
-  <autoFilter ref="B2:M7" xr:uid="{C4B251E0-643A-4206-BBF7-CC749B7A14EB}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD3A9504-19FF-431D-AD02-E3A18E1E6005}" name="Table4" displayName="Table4" ref="B2:K7" totalsRowShown="0">
+  <autoFilter ref="B2:K7" xr:uid="{C4B251E0-643A-4206-BBF7-CC749B7A14EB}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{BBD2AB90-330C-4889-9F93-EDB3DAC75598}" name="CourseId"/>
     <tableColumn id="2" xr3:uid="{6A1266B7-5B89-43F6-80A7-B7A60A4EDE36}" name="CourseTitle"/>
-    <tableColumn id="3" xr3:uid="{63BD42BA-3A9F-4A5B-BC44-A515C7B56454}" name="StartDate" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{E7910765-FC85-408B-AF0E-FF4C19341063}" name="EndDate" dataDxfId="15"/>
     <tableColumn id="5" xr3:uid="{29E60449-D205-475F-B9B0-23F9F289014D}" name="MinEnrolled" dataDxfId="14"/>
     <tableColumn id="6" xr3:uid="{7E87158C-1ABB-4BE4-BE25-21E7D2F5E5DE}" name="MaxEnrolled" dataDxfId="13"/>
     <tableColumn id="7" xr3:uid="{0CAB1DCC-E7F9-43AE-B2D2-575593066633}" name="PriceGroupId" dataDxfId="12"/>
     <tableColumn id="8" xr3:uid="{28D4FECB-89DB-4C4A-80BA-6206B53E0C57}" name="CourseLevelId" dataDxfId="11"/>
     <tableColumn id="9" xr3:uid="{AAAEBDA5-7F1F-4E34-930D-B59FE7D33A88}" name="EnrollmentModeId" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{768D8BDA-3017-44F8-A1BD-9736C92BD7B4}" name="Id" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{13244F1B-2EE0-4064-87DE-B6694040B439}" name="Result" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{59D66F19-790F-4E1B-A5C4-E14C8BD8F0C9}" name="Reason" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{DD147660-E588-4F89-A162-7E559389E4FD}" name="Id" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{510FE357-5F8C-4AA5-9627-D47E4672B923}" name="Result" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{3B056C32-BE6D-493F-810D-5268E6114737}" name="Error" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -924,17 +843,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB64985A-CB9C-4DF2-B5A4-57E870AE0968}" name="Table2" displayName="Table2" ref="A2:K7" totalsRowShown="0">
   <autoFilter ref="A2:K7" xr:uid="{032F4120-5C68-48FC-84AE-4CFAC05B379F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{3BF69D39-73BE-41DA-8B4C-1BE55B6A2B1B}" name="Column1"/>
-    <tableColumn id="11" xr3:uid="{1CBA23AA-8C4F-45AE-A99B-3FC6B863D6ED}" name="CourseId"/>
+    <tableColumn id="1" xr3:uid="{3BF69D39-73BE-41DA-8B4C-1BE55B6A2B1B}" name="CourseId"/>
+    <tableColumn id="11" xr3:uid="{1CBA23AA-8C4F-45AE-A99B-3FC6B863D6ED}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{79B32707-32F4-4BC4-BAA6-20D35B19667B}" name="AcademicPeriod"/>
     <tableColumn id="3" xr3:uid="{7BC7B7A3-B7CF-4873-AF6F-0C2BF70E766E}" name="CourseTitle"/>
-    <tableColumn id="4" xr3:uid="{292610B1-17A8-4CA8-BCE1-2FEAD6F80957}" name="StartDate" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{65618288-7FF0-49AF-866C-85402153928E}" name="EndDate" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{E03D4FEA-D895-44A4-AAE3-067447E43FDC}" name="MinEnrolled" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{5DEFECE5-5E57-4AB6-AE82-A308296B781C}" name="MaxEnrolled" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{552CB59F-DDEF-4CD4-9D23-3DCC91131D5F}" name="PriceGroupId" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{62F30E08-B401-41D0-A31F-202E30BDF563}" name="CourselevelId" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{41A3505F-3B98-44FB-B699-E7D27E5E771D}" name="EnrollmentModeId" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{292610B1-17A8-4CA8-BCE1-2FEAD6F80957}" name="StartDate" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{65618288-7FF0-49AF-866C-85402153928E}" name="EndDate" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{E03D4FEA-D895-44A4-AAE3-067447E43FDC}" name="MinEnrolled" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{5DEFECE5-5E57-4AB6-AE82-A308296B781C}" name="MaxEnrolled" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{552CB59F-DDEF-4CD4-9D23-3DCC91131D5F}" name="PriceGroupId" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{62F30E08-B401-41D0-A31F-202E30BDF563}" name="CourselevelId" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{41A3505F-3B98-44FB-B699-E7D27E5E771D}" name="EnrollmentModeId" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1303,26 +1222,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8856C5D-B3C7-4426-8B6F-58530CABC3AA}">
-  <dimension ref="B2:M7"/>
+  <dimension ref="B2:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="17.1796875" customWidth="1"/>
     <col min="3" max="3" width="59.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" customWidth="1"/>
-    <col min="8" max="8" width="33" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
-    <col min="10" max="10" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -1338,187 +1255,151 @@
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" t="s">
-        <v>51</v>
-      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="8">
-        <v>44408</v>
-      </c>
-      <c r="F3" s="1">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="E4" s="1">
         <v>9999</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9999</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9999</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="8">
-        <v>44044</v>
-      </c>
-      <c r="E4" s="8">
-        <v>44408</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="H6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="6">
         <v>0</v>
       </c>
-      <c r="G4" s="1">
+      <c r="E7" s="6">
         <v>9999</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8">
-        <v>44044</v>
-      </c>
-      <c r="E5" s="8">
-        <v>44408</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>9999</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="8">
-        <v>44044</v>
-      </c>
-      <c r="E6" s="8">
-        <v>44408</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>9999</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="8">
-        <v>44044</v>
-      </c>
-      <c r="E7" s="8">
-        <v>44408</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>9999</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="F7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1533,13 +1414,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DCD2C6-0ECE-4E12-8333-40826AC775D9}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="23.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
     <col min="3" max="3" width="29.54296875" customWidth="1"/>
     <col min="4" max="4" width="38.453125" customWidth="1"/>
     <col min="5" max="5" width="10.81640625" customWidth="1"/>
@@ -1553,7 +1434,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1">
         <v>529</v>
@@ -1577,52 +1458,52 @@
         <v>563</v>
       </c>
       <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
         <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+      <c r="A3" t="s">
         <v>39</v>
       </c>
       <c r="C3" t="s">
@@ -1631,154 +1512,154 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="9">
+      <c r="E3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="8">
         <v>0</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>9999</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>20</v>
+      <c r="I3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="9">
+      <c r="E4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>9999</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>20</v>
+      <c r="I4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>43</v>
+      <c r="A5" t="s">
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="9">
+        <v>46</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>9999</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>20</v>
+      <c r="I5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>43</v>
+      <c r="A6" t="s">
+        <v>44</v>
       </c>
       <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>9999</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="9">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9">
-        <v>9999</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>20</v>
+      <c r="J6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>43</v>
+      <c r="A7" t="s">
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="9">
+        <v>46</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>9999</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>20</v>
+      <c r="I7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1791,6 +1672,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D4E4CE400B31F49832066229853696E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="445a960a3078ae26e39021af810f1ecd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1fb4680b-a77b-4fa6-8abd-f629a05f0edb" xmlns:ns3="be28adde-14b9-4448-abf4-cd7ec8b9ea5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad286e4f30d99469e05d6eedfa6a12d0" ns2:_="" ns3:_="">
     <xsd:import namespace="1fb4680b-a77b-4fa6-8abd-f629a05f0edb"/>
@@ -1993,22 +1889,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E5614E-0934-4955-A586-47AD85CBCA55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB619A27-B152-46DC-82C3-E0ECE583C032}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13AC6F4A-2A37-46B6-9F53-1A3F9CFBF02B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2025,21 +1923,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E5614E-0934-4955-A586-47AD85CBCA55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB619A27-B152-46DC-82C3-E0ECE583C032}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
end to end changeset
</commit_message>
<xml_diff>
--- a/UpdateCourseOfferingCourseOfferingTemplate.xlsx
+++ b/UpdateCourseOfferingCourseOfferingTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Venkat\Git\ExcelUpload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Venkat\Source\ExcelUpload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1B95AC-C021-4B81-ACB2-9C25C47751E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4897CEA3-918B-43B5-B6E7-B1956ACFE68B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="7590" firstSheet="1" activeTab="1" xr2:uid="{DC0DE665-DC5B-4E82-A28B-EA52864D6C96}"/>
   </bookViews>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8856C5D-B3C7-4426-8B6F-58530CABC3AA}">
   <dimension ref="B2:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1276,7 +1276,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
         <v>9999</v>
@@ -1302,10 +1302,10 @@
         <v>19</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1">
-        <v>9999</v>
+        <v>9998</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>20</v>
@@ -1328,10 +1328,10 @@
         <v>23</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>9999</v>
+        <v>9997</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
@@ -1354,10 +1354,10 @@
         <v>26</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>9999</v>
+        <v>9996</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>20</v>
@@ -1379,11 +1379,9 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="6">
-        <v>9999</v>
+        <v>99995</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>20</v>
@@ -1669,6 +1667,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D4E4CE400B31F49832066229853696E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="445a960a3078ae26e39021af810f1ecd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1fb4680b-a77b-4fa6-8abd-f629a05f0edb" xmlns:ns3="be28adde-14b9-4448-abf4-cd7ec8b9ea5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad286e4f30d99469e05d6eedfa6a12d0" ns2:_="" ns3:_="">
     <xsd:import namespace="1fb4680b-a77b-4fa6-8abd-f629a05f0edb"/>
@@ -1871,22 +1884,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E5614E-0934-4955-A586-47AD85CBCA55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB619A27-B152-46DC-82C3-E0ECE583C032}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13AC6F4A-2A37-46B6-9F53-1A3F9CFBF02B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1903,21 +1918,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB619A27-B152-46DC-82C3-E0ECE583C032}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E5614E-0934-4955-A586-47AD85CBCA55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>